<commit_message>
adding the mat files
</commit_message>
<xml_diff>
--- a/em.xlsx
+++ b/em.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\study staff\share\arielmichaelshare\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DAC4A06-50A7-410C-9E04-DB9BAFC63A2C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCBAFA9C-F4BF-4CD0-AB7C-B8AF59EF515C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="680" windowWidth="2370" windowHeight="560" activeTab="4" xr2:uid="{1276EE7E-AA85-41CB-94EC-3C468A4BC312}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{1276EE7E-AA85-41CB-94EC-3C468A4BC312}"/>
   </bookViews>
   <sheets>
     <sheet name="ניסוי 1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>זרם</t>
   </si>
@@ -101,6 +101,15 @@
   </si>
   <si>
     <t>delta B</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>delta y</t>
+  </si>
+  <si>
+    <t>I</t>
   </si>
 </sst>
 </file>
@@ -136,8 +145,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1383,10 +1395,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3FFA141-5AA6-4FB1-B946-CCDAAECE68F0}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1394,12 +1406,14 @@
     <col min="1" max="1" width="12.26953125" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" customWidth="1"/>
+    <col min="4" max="4" width="11.1796875" customWidth="1"/>
     <col min="5" max="5" width="11.54296875" customWidth="1"/>
     <col min="6" max="6" width="27.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31" customWidth="1"/>
+    <col min="8" max="8" width="11.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -1415,108 +1429,170 @@
       <c r="E1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>24.2</v>
+        <f>D16-4.5</f>
+        <v>19.7</v>
       </c>
       <c r="B2">
         <v>14.1</v>
       </c>
       <c r="C2">
         <f>A2-4.5</f>
-        <v>19.7</v>
+        <v>15.2</v>
       </c>
       <c r="D2">
         <f>2*10^-7*(0.205)^2*0.5*130/(((A2/100)^2+(0.205/2)^2)*SQRT((A2/100)^2+2*(0.205/2)^2))</f>
-        <v>2.803932984932202E-5</v>
+        <v>4.5294053218696631E-5</v>
       </c>
       <c r="E2">
         <f>4*PI()*10^-7/(2*PI())*SQRT(((0.205^2*130*0.01)/(((A2/100)^2+(0.205/2)^2)*SQRT((A2/100)^2+2*(0.205/2)^2)))^2+((2*0.205*(A2/100)^2*130*0.5*0.005)/(((A2/100)^2+(0.205/2)^2)*((A2/100)^2+2*(0.205/2)^2)^(3/2)))^2+((0.205^2*130*0.5*(4*(A2/100)^3+(5/4)*0.205^2)*0.1)/(((A2/100)^2+(0.205/2)^2)^2*SQRT((A2/100)^2+2*(0.205/2)^2)))^2)</f>
-        <v>4.5811565415104069E-6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+        <v>7.8196268591891185E-6</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2">
+        <f>(2*PI()/(B2/20))^2*7.41927*10^-7</f>
+        <v>5.8930846412047879E-5</v>
+      </c>
+      <c r="H2">
+        <f>4*PI()^2*SQRT((5.37712*10^-8/(B2/20)^2)^2+(2*7.41927*10^-7*0.025/(B2/20)^3)^2)</f>
+        <v>5.9757626528744854E-6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>22</v>
+        <f>D17-4.5</f>
+        <v>17.5</v>
       </c>
       <c r="B3">
         <v>13</v>
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C11" si="0">A3-4.5</f>
-        <v>17.5</v>
+        <v>13</v>
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D11" si="1">2*10^-7*(0.205)^2*0.5*130/(((A3/100)^2+(0.205/2)^2)*SQRT((A3/100)^2+2*(0.205/2)^2))</f>
-        <v>3.520228502151322E-5</v>
+        <v>5.8451621352159964E-5</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E11" si="2">4*PI()*10^-7/(2*PI())*SQRT(((0.205^2*130*0.01)/(((A3/100)^2+(0.205/2)^2)*SQRT((A3/100)^2+2*(0.205/2)^2)))^2+((2*0.205*(A3/100)^2*130*0.5*0.005)/(((A3/100)^2+(0.205/2)^2)*((A3/100)^2+2*(0.205/2)^2)^(3/2)))^2+((0.205^2*130*0.5*(4*(A3/100)^3+(5/4)*0.205^2)*0.1)/(((A3/100)^2+(0.205/2)^2)^2*SQRT((A3/100)^2+2*(0.205/2)^2)))^2)</f>
-        <v>5.8517920019310922E-6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+        <v>1.0710839086390667E-5</v>
+      </c>
+      <c r="F3">
+        <f>5.5/1000*((4/100)^2/12+(0.25/100)^2/4)</f>
+        <v>7.4192708333333323E-7</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G11" si="3">(2*PI()/(B3/20))^2*7.41927*10^-7</f>
+        <v>6.9325689793959966E-5</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H6" si="4">4*PI()^2*SQRT((5.37712*10^-8/(B3/20)^2)^2+(2*7.41927*10^-7*0.025/(B3/20)^3)^2)</f>
+        <v>7.3268410240643233E-6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>19</v>
+        <f t="shared" ref="A4:A6" si="5">D18-4.5</f>
+        <v>14.5</v>
       </c>
       <c r="B4">
         <v>11.58</v>
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>14.5</v>
+        <v>10</v>
       </c>
       <c r="D4">
         <f t="shared" si="1"/>
-        <v>4.9050261657003193E-5</v>
+        <v>8.4506759070164465E-5</v>
       </c>
       <c r="E4">
         <f t="shared" si="2"/>
-        <v>8.6069694261195627E-6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+        <v>1.7550780909894349E-5</v>
+      </c>
+      <c r="F4">
+        <f>SQRT(((5.5/1000)*4/100/6*0.01/100)^2+(5.5/1000*0.25/100/2*0.002/100)^2+(((4/100)^2/6+(0.25/100)^2/4)*(0.2/1000))^2 )</f>
+        <v>5.3771170572363615E-8</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="3"/>
+        <v>8.7370291634818222E-5</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="4"/>
+        <v>9.8499901742052275E-6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>16</v>
+        <f t="shared" si="5"/>
+        <v>11.5</v>
       </c>
       <c r="B5">
         <v>10</v>
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>11.5</v>
+        <v>7</v>
       </c>
       <c r="D5">
         <f t="shared" si="1"/>
-        <v>7.0083775754163299E-5</v>
+        <v>1.244169175162409E-4</v>
       </c>
       <c r="E5">
         <f t="shared" si="2"/>
-        <v>1.3580403070055191E-5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+        <v>3.0919806760903288E-5</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="3"/>
+        <v>1.1716041575179238E-4</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="4"/>
+        <v>1.4469493285155731E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>13</v>
+        <f t="shared" si="5"/>
+        <v>8.5</v>
       </c>
       <c r="B6">
         <v>8.57</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>8.5</v>
+        <v>4</v>
       </c>
       <c r="D6">
         <f t="shared" si="1"/>
-        <v>1.0237885019080932E-4</v>
+        <v>1.8335746639464883E-4</v>
       </c>
       <c r="E6">
         <f t="shared" si="2"/>
-        <v>2.3105262025829036E-5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+        <v>5.7026467749683725E-5</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="3"/>
+        <v>1.5952151306869826E-4</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="4"/>
+        <v>2.1912173064197792E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -1528,8 +1604,16 @@
         <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G7" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H7" t="e">
+        <f t="shared" ref="H3:H11" si="6">4*PI()^2*SQRT((5.37712*10^-8/(B7/20)^2)^2+(2*7.41927*10^-7*0.2/(B7/20)^3)^2)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>16</v>
       </c>
@@ -1548,8 +1632,16 @@
         <f t="shared" si="2"/>
         <v>1.3580403070055191E-5</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G8">
+        <f t="shared" si="3"/>
+        <v>1.2451951934508703E-4</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="6"/>
+        <v>1.0309226932943886E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>19</v>
       </c>
@@ -1568,8 +1660,16 @@
         <f t="shared" si="2"/>
         <v>8.6069694261195627E-6</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G9">
+        <f t="shared" si="3"/>
+        <v>9.0151135543084282E-5</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="6"/>
+        <v>6.3600450622731798E-5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>22</v>
       </c>
@@ -1588,8 +1688,16 @@
         <f t="shared" si="2"/>
         <v>5.8517920019310922E-6</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G10">
+        <f t="shared" si="3"/>
+        <v>6.8480262459080546E-5</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="6"/>
+        <v>4.217698367387886E-5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>24.2</v>
       </c>
@@ -1608,18 +1716,93 @@
         <f t="shared" si="2"/>
         <v>4.5811565415104069E-6</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G11">
+        <f t="shared" si="3"/>
+        <v>5.8764021735886035E-5</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="6"/>
+        <v>3.3565355644565306E-5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>17</v>
       </c>
       <c r="B13">
         <v>22</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C13">
+        <f>B13/20</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F13">
+        <f>B2/20</f>
+        <v>0.70499999999999996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C14">
+        <f>0.2/20</f>
+        <v>0.01</v>
+      </c>
+      <c r="F14">
+        <f t="shared" ref="F14:F20" si="7">B3/20</f>
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>12</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="7"/>
+        <v>0.57899999999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D16">
+        <v>24.2</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="7"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D17">
+        <v>22</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="7"/>
+        <v>0.42849999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D18">
+        <v>19</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D19">
+        <v>16</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="7"/>
+        <v>0.48499999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D20">
+        <v>13</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="7"/>
+        <v>0.57000000000000006</v>
       </c>
     </row>
   </sheetData>

</xml_diff>